<commit_message>
rollAvg:  latest spreadsheet from Dave
</commit_message>
<xml_diff>
--- a/apps/rollAvgApp/doc/ESR_HALLS_Cryo_Overview.xlsx
+++ b/apps/rollAvgApp/doc/ESR_HALLS_Cryo_Overview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="566">
   <si>
     <t>Parameters of ESR and Halls A, B, and C to help operators to understand the complete system, its status and effect of your changes on others</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Revision</t>
   </si>
   <si>
-    <t>1_3</t>
+    <t>1_5</t>
   </si>
   <si>
     <t>Date</t>
@@ -160,7 +160,7 @@
     <t>4 atm Helium warm gas to Hall A DBX</t>
   </si>
   <si>
-    <t>FI8561</t>
+    <t>B_TORUS:LHe:FI8561_Flow</t>
   </si>
   <si>
     <t>4atm warm He to Hall B</t>
@@ -820,13 +820,13 @@
     <t>Solenoid VCL flow B</t>
   </si>
   <si>
-    <t>B_SOL:LHe:PV8522SR</t>
+    <t>B_TORUS:LHe:PV8522SR</t>
   </si>
   <si>
     <t>Solenoid cold return valve</t>
   </si>
   <si>
-    <t>B_SOL:LHe:PV8522SCD</t>
+    <t>B_TORUS:LHe:PV8522SCD</t>
   </si>
   <si>
     <t>Solenoid warm return valve</t>
@@ -982,55 +982,55 @@
     <t>Hall C Magnets and Target </t>
   </si>
   <si>
-    <t>ecQ1_H_LHe</t>
+    <t>ecQ1_h_LHe</t>
   </si>
   <si>
     <t>Helium level HMS Q1</t>
   </si>
   <si>
-    <t>ecQ2_H_LHe</t>
+    <t>ecQ2_h_LHe</t>
   </si>
   <si>
     <t>Helium level HMS Q2</t>
   </si>
   <si>
-    <t>ecQ3_H_LHe</t>
+    <t>ecQ3_h_LHe</t>
   </si>
   <si>
     <t>Helium level HMS Q3</t>
   </si>
   <si>
-    <t>ecDI_H_LHe</t>
+    <t>ecDI_h_LHe</t>
   </si>
   <si>
     <t>Helium level HMS Dipole</t>
   </si>
   <si>
-    <t>ecSHB_H_LHe</t>
+    <t>ecSHB_h_LHe</t>
   </si>
   <si>
     <t>Helium level  SHMS HB</t>
   </si>
   <si>
-    <t>ecSQ1_H_LHe</t>
+    <t>ecSQ1_h_LHe</t>
   </si>
   <si>
     <t>Helium level  SHMS Q1</t>
   </si>
   <si>
-    <t>ecSQ2_H_LHe</t>
+    <t>ecSQ2_h_LHe</t>
   </si>
   <si>
     <t>Helium level  SHMS Q2</t>
   </si>
   <si>
-    <t>ecSQ3_H_LHe</t>
+    <t>ecSQ3_h_LHe</t>
   </si>
   <si>
     <t>Helium level  SHMS Q3</t>
   </si>
   <si>
-    <t>ecSDI_H_LHe</t>
+    <t>ecSDI_h_LHe</t>
   </si>
   <si>
     <t>Helium level  SHMS Dipole</t>
@@ -1207,7 +1207,7 @@
     <t>SHMS Dipole VCL - Flow</t>
   </si>
   <si>
-    <t>ecDI_V5_LVDT_true</t>
+    <t>ecDI_S5_LVDT_true</t>
   </si>
   <si>
     <t>HMS DI 4K Supply Valve</t>
@@ -1231,7 +1231,7 @@
     <t>HMS Q1 4K Supply Valve</t>
   </si>
   <si>
-    <t>ecDI_V6_LVDT_true</t>
+    <t>ecDI_S6_LVDT_true</t>
   </si>
   <si>
     <t>HMS DI 4K Return Valve</t>
@@ -1279,61 +1279,61 @@
     <t>HMS Q1 Warm Return Valve</t>
   </si>
   <si>
-    <t>ecSDI_S5_LVDT_true</t>
+    <t>ecSDI_V5_LVDT_true</t>
   </si>
   <si>
     <t>SHMS DI 4K Supply Valve</t>
   </si>
   <si>
-    <t>ecSQ3_S5_LVDT_true</t>
+    <t>ecSQ3_V5_LVDT_true</t>
   </si>
   <si>
     <t>SHMS Q3 4K Supply Valve</t>
   </si>
   <si>
-    <t>ecSQ2_S5_LVDT_true</t>
+    <t>ecSQ2_V5_LVDT_true</t>
   </si>
   <si>
     <t>SHMS Q2 4K Supply Valve</t>
   </si>
   <si>
-    <t>ecSQ1_S5_LVDT_true</t>
+    <t>ecSQ1_V5_LVDT_true</t>
   </si>
   <si>
     <t>SHMS Q1 4K Supply Valve</t>
   </si>
   <si>
-    <t>ecSHB_S5_LVDT_true</t>
+    <t>ecSHB_V5_LVDT_true</t>
   </si>
   <si>
     <t>SHMS HB 4K Supply Valve</t>
   </si>
   <si>
-    <t>ecSDI_S6_LVDT_true</t>
+    <t>ecSDI_V6_LVDT_true</t>
   </si>
   <si>
     <t>SHMS DI 4K Return Valve</t>
   </si>
   <si>
-    <t>ecSQ3_S6_LVDT_true</t>
+    <t>ecSQ3_V6_LVDT_true</t>
   </si>
   <si>
     <t>SHMS Q3 4K Return Valve</t>
   </si>
   <si>
-    <t>ecSQ2_S6_LVDT_true</t>
+    <t>ecSQ2_V6_LVDT_true</t>
   </si>
   <si>
     <t>SHMS Q2 4K Return Valve</t>
   </si>
   <si>
-    <t>ecSQ1_S6_LVDT_true</t>
+    <t>ecSQ1_V6_LVDT_true</t>
   </si>
   <si>
     <t>SHMS Q1 4K Return Valve</t>
   </si>
   <si>
-    <t>ecSHB_S6_LVDT_true</t>
+    <t>ecSHB_V6_LVDT_true</t>
   </si>
   <si>
     <t>SHMS HB 4K Return Valve</t>
@@ -1369,7 +1369,7 @@
     <t>SHMS HB Warm Return Valve</t>
   </si>
   <si>
-    <t>CEV6711C.ORBC</t>
+    <t>CEV6711C.ORBV</t>
   </si>
   <si>
     <t>Cryo's 4K Supply Valve to Hall C</t>
@@ -1712,6 +1712,12 @@
   </si>
   <si>
     <t>beam current on Hall C cryotarget</t>
+  </si>
+  <si>
+    <t>UPDATED 10_30_17</t>
+  </si>
+  <si>
+    <t>Seem to be correct already 10_30_17</t>
   </si>
 </sst>
 </file>
@@ -1762,7 +1768,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1785,6 +1791,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B4"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -1822,7 +1834,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1859,16 +1871,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1896,6 +1912,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1953,7 +1973,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -1976,17 +1996,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L298"/>
+  <dimension ref="A1:L304"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A206" activeCellId="0" sqref="A206"/>
+      <selection pane="bottomLeft" activeCell="C145" activeCellId="0" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8826530612245"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.3877551020408"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.8163265306122"/>
@@ -2023,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>43025</v>
+        <v>43040</v>
       </c>
       <c r="C4" s="5"/>
       <c r="E4" s="5"/>
@@ -2260,7 +2280,7 @@
       <c r="L16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -3008,7 +3028,7 @@
       <c r="B61" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="13" t="s">
         <v>149</v>
       </c>
       <c r="E61" s="1" t="n">
@@ -3419,7 +3439,7 @@
       <c r="L82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="12" t="s">
+      <c r="A83" s="13" t="s">
         <v>197</v>
       </c>
       <c r="B83" s="0" t="s">
@@ -3437,7 +3457,7 @@
       <c r="L83" s="0"/>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="12" t="s">
+      <c r="A84" s="13" t="s">
         <v>199</v>
       </c>
       <c r="B84" s="0" t="s">
@@ -3455,7 +3475,7 @@
       <c r="L84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="13" t="s">
         <v>201</v>
       </c>
       <c r="B85" s="0" t="s">
@@ -3473,7 +3493,7 @@
       <c r="L85" s="0"/>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="12" t="s">
+      <c r="A86" s="13" t="s">
         <v>203</v>
       </c>
       <c r="B86" s="0" t="s">
@@ -3491,7 +3511,7 @@
       <c r="L86" s="0"/>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="12" t="s">
+      <c r="A87" s="13" t="s">
         <v>205</v>
       </c>
       <c r="B87" s="0" t="s">
@@ -3509,7 +3529,7 @@
       <c r="L87" s="0"/>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="12" t="s">
+      <c r="A88" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B88" s="0" t="s">
@@ -3527,7 +3547,7 @@
       <c r="L88" s="0"/>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="12" t="s">
+      <c r="A89" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B89" s="0" t="s">
@@ -3545,7 +3565,7 @@
       <c r="L89" s="0"/>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="13" t="s">
         <v>211</v>
       </c>
       <c r="B90" s="0" t="s">
@@ -3565,7 +3585,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="12" t="s">
+      <c r="A91" s="13" t="s">
         <v>214</v>
       </c>
       <c r="B91" s="0" t="s">
@@ -3583,7 +3603,7 @@
       <c r="L91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="12" t="s">
+      <c r="A92" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B92" s="0" t="s">
@@ -3601,7 +3621,7 @@
       <c r="L92" s="0"/>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="12" t="s">
+      <c r="A93" s="13" t="s">
         <v>218</v>
       </c>
       <c r="B93" s="0" t="s">
@@ -3619,7 +3639,7 @@
       <c r="L93" s="0"/>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="12" t="s">
+      <c r="A94" s="13" t="s">
         <v>220</v>
       </c>
       <c r="B94" s="0" t="s">
@@ -3637,7 +3657,7 @@
       <c r="L94" s="0"/>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="12" t="s">
+      <c r="A95" s="13" t="s">
         <v>222</v>
       </c>
       <c r="B95" s="0" t="s">
@@ -3655,7 +3675,7 @@
       <c r="L95" s="0"/>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="12" t="s">
+      <c r="A96" s="13" t="s">
         <v>224</v>
       </c>
       <c r="B96" s="0" t="s">
@@ -3675,7 +3695,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="13" t="s">
         <v>226</v>
       </c>
       <c r="B97" s="0" t="s">
@@ -3693,7 +3713,7 @@
       <c r="L97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="13" t="s">
         <v>228</v>
       </c>
       <c r="B98" s="0" t="s">
@@ -3711,7 +3731,7 @@
       <c r="L98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="12" t="s">
+      <c r="A99" s="13" t="s">
         <v>230</v>
       </c>
       <c r="B99" s="0" t="s">
@@ -3729,7 +3749,7 @@
       <c r="L99" s="0"/>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="12" t="s">
+      <c r="A100" s="13" t="s">
         <v>232</v>
       </c>
       <c r="B100" s="0" t="s">
@@ -3747,7 +3767,7 @@
       <c r="L100" s="0"/>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="12" t="s">
+      <c r="A101" s="13" t="s">
         <v>234</v>
       </c>
       <c r="B101" s="0" t="s">
@@ -3765,7 +3785,7 @@
       <c r="L101" s="0"/>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="12" t="s">
+      <c r="A102" s="13" t="s">
         <v>236</v>
       </c>
       <c r="B102" s="0" t="s">
@@ -3977,8 +3997,11 @@
       <c r="L115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+      <c r="A116" s="12" t="s">
         <v>266</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>267</v>
@@ -3995,8 +4018,11 @@
       <c r="L116" s="0"/>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="A117" s="12" t="s">
         <v>268</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>269</v>
@@ -4177,6 +4203,9 @@
       <c r="A127" s="0" t="s">
         <v>293</v>
       </c>
+      <c r="B127" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="C127" s="0" t="s">
         <v>294</v>
       </c>
@@ -4195,6 +4224,9 @@
       <c r="A128" s="0" t="s">
         <v>295</v>
       </c>
+      <c r="B128" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="C128" s="0" t="s">
         <v>296</v>
       </c>
@@ -4340,7 +4372,7 @@
       <c r="L137" s="0"/>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
+      <c r="A138" s="12" t="s">
         <v>320</v>
       </c>
       <c r="B138" s="0" t="s">
@@ -4358,7 +4390,7 @@
       <c r="L138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+      <c r="A139" s="12" t="s">
         <v>322</v>
       </c>
       <c r="B139" s="0" t="s">
@@ -4376,7 +4408,7 @@
       <c r="L139" s="0"/>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+      <c r="A140" s="12" t="s">
         <v>324</v>
       </c>
       <c r="B140" s="0" t="s">
@@ -4394,7 +4426,7 @@
       <c r="L140" s="0"/>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
+      <c r="A141" s="12" t="s">
         <v>326</v>
       </c>
       <c r="B141" s="0" t="s">
@@ -4412,7 +4444,7 @@
       <c r="L141" s="0"/>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
+      <c r="A142" s="12" t="s">
         <v>328</v>
       </c>
       <c r="B142" s="0" t="s">
@@ -4430,7 +4462,7 @@
       <c r="L142" s="0"/>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
+      <c r="A143" s="12" t="s">
         <v>330</v>
       </c>
       <c r="B143" s="0" t="s">
@@ -4448,7 +4480,7 @@
       <c r="L143" s="0"/>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
+      <c r="A144" s="12" t="s">
         <v>332</v>
       </c>
       <c r="B144" s="0" t="s">
@@ -4466,7 +4498,7 @@
       <c r="L144" s="0"/>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
+      <c r="A145" s="12" t="s">
         <v>334</v>
       </c>
       <c r="B145" s="0" t="s">
@@ -4484,7 +4516,7 @@
       <c r="L145" s="0"/>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+      <c r="A146" s="12" t="s">
         <v>336</v>
       </c>
       <c r="B146" s="0" t="s">
@@ -5027,7 +5059,7 @@
       <c r="L174" s="0"/>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="0" t="s">
+      <c r="A175" s="12" t="s">
         <v>395</v>
       </c>
       <c r="D175" s="0" t="s">
@@ -5066,7 +5098,7 @@
       <c r="L179" s="0"/>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
+      <c r="A180" s="12" t="s">
         <v>403</v>
       </c>
       <c r="D180" s="0" t="s">
@@ -5144,7 +5176,7 @@
       <c r="L189" s="0"/>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="0" t="s">
+      <c r="A190" s="12" t="s">
         <v>419</v>
       </c>
       <c r="D190" s="0" t="s">
@@ -5153,7 +5185,7 @@
       <c r="L190" s="0"/>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="s">
+      <c r="A191" s="12" t="s">
         <v>421</v>
       </c>
       <c r="D191" s="0" t="s">
@@ -5162,7 +5194,7 @@
       <c r="L191" s="0"/>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
+      <c r="A192" s="12" t="s">
         <v>423</v>
       </c>
       <c r="D192" s="0" t="s">
@@ -5171,7 +5203,7 @@
       <c r="L192" s="0"/>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="s">
+      <c r="A193" s="12" t="s">
         <v>425</v>
       </c>
       <c r="D193" s="0" t="s">
@@ -5180,7 +5212,7 @@
       <c r="L193" s="0"/>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="s">
+      <c r="A194" s="12" t="s">
         <v>427</v>
       </c>
       <c r="D194" s="0" t="s">
@@ -5192,7 +5224,7 @@
       <c r="L195" s="0"/>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="0" t="s">
+      <c r="A196" s="12" t="s">
         <v>429</v>
       </c>
       <c r="D196" s="0" t="s">
@@ -5201,7 +5233,7 @@
       <c r="L196" s="0"/>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="0" t="s">
+      <c r="A197" s="12" t="s">
         <v>431</v>
       </c>
       <c r="D197" s="0" t="s">
@@ -5210,7 +5242,7 @@
       <c r="L197" s="0"/>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="0" t="s">
+      <c r="A198" s="12" t="s">
         <v>433</v>
       </c>
       <c r="D198" s="0" t="s">
@@ -5219,7 +5251,7 @@
       <c r="L198" s="0"/>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="0" t="s">
+      <c r="A199" s="12" t="s">
         <v>435</v>
       </c>
       <c r="D199" s="0" t="s">
@@ -5228,7 +5260,7 @@
       <c r="L199" s="0"/>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="s">
+      <c r="A200" s="12" t="s">
         <v>437</v>
       </c>
       <c r="D200" s="0" t="s">
@@ -5321,7 +5353,7 @@
       <c r="L218" s="0"/>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="0" t="s">
+      <c r="A219" s="12" t="s">
         <v>449</v>
       </c>
       <c r="B219" s="0" t="s">
@@ -5548,27 +5580,27 @@
       <c r="L235" s="0"/>
     </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="13" t="s">
+      <c r="A243" s="14" t="s">
         <v>480</v>
       </c>
-      <c r="B243" s="14"/>
-      <c r="C243" s="14"/>
-      <c r="D243" s="14"/>
+      <c r="B243" s="15"/>
+      <c r="C243" s="15"/>
+      <c r="D243" s="15"/>
       <c r="E243" s="0"/>
       <c r="F243" s="0"/>
       <c r="L243" s="0"/>
     </row>
     <row r="244" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="15" t="s">
+      <c r="A244" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B244" s="15"/>
-      <c r="C244" s="15"/>
-      <c r="D244" s="15"/>
-      <c r="E244" s="16" t="s">
+      <c r="B244" s="16"/>
+      <c r="C244" s="16"/>
+      <c r="D244" s="16"/>
+      <c r="E244" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F244" s="16" t="s">
+      <c r="F244" s="17" t="s">
         <v>11</v>
       </c>
       <c r="G244" s="3" t="s">
@@ -6017,27 +6049,27 @@
       <c r="L269" s="0"/>
     </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="17" t="s">
+      <c r="A272" s="18" t="s">
         <v>536</v>
       </c>
-      <c r="B272" s="18"/>
-      <c r="C272" s="18"/>
-      <c r="D272" s="18"/>
+      <c r="B272" s="19"/>
+      <c r="C272" s="19"/>
+      <c r="D272" s="19"/>
       <c r="E272" s="0"/>
       <c r="F272" s="0"/>
       <c r="L272" s="0"/>
     </row>
     <row r="273" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="15" t="s">
+      <c r="A273" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B273" s="15"/>
-      <c r="C273" s="15"/>
-      <c r="D273" s="15"/>
-      <c r="E273" s="16" t="s">
+      <c r="B273" s="16"/>
+      <c r="C273" s="16"/>
+      <c r="D273" s="16"/>
+      <c r="E273" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F273" s="16" t="s">
+      <c r="F273" s="17" t="s">
         <v>11</v>
       </c>
       <c r="G273" s="3" t="s">
@@ -6485,6 +6517,16 @@
       </c>
       <c r="D298" s="0" t="s">
         <v>563</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="12" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="20" t="s">
+        <v>565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ESR_HALLS_Cryo*:  fix label swaps
</commit_message>
<xml_diff>
--- a/apps/rollAvgApp/doc/ESR_HALLS_Cryo_Overview.xlsx
+++ b/apps/rollAvgApp/doc/ESR_HALLS_Cryo_Overview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1258,27 +1258,27 @@
     <t>ecQ1_vWR_LVDT_true</t>
   </si>
   <si>
+    <t>HMS Q1 Warm Return Valve</t>
+  </si>
+  <si>
+    <t>ecQ2_vWR_LVDT_true</t>
+  </si>
+  <si>
+    <t>HMS Q2 Warm Return Valve</t>
+  </si>
+  <si>
+    <t>ecQ3_vWR_LVDT_true</t>
+  </si>
+  <si>
+    <t>HMS Q3 Warm Return Valve</t>
+  </si>
+  <si>
+    <t>ecDI_s11_LVDT_true</t>
+  </si>
+  <si>
     <t>HMS DI Warm Return Valve</t>
   </si>
   <si>
-    <t>ecQ2_vWR_LVDT_true</t>
-  </si>
-  <si>
-    <t>HMS Q3 Warm Return Valve</t>
-  </si>
-  <si>
-    <t>ecQ3_vWR_LVDT_true</t>
-  </si>
-  <si>
-    <t>HMS Q2 Warm Return Valve</t>
-  </si>
-  <si>
-    <t>ecDI_s11_LVDT_true</t>
-  </si>
-  <si>
-    <t>HMS Q1 Warm Return Valve</t>
-  </si>
-  <si>
     <t>ecSDI_V5_LVDT_true</t>
   </si>
   <si>
@@ -1348,25 +1348,25 @@
     <t>ecSHB_vWR_LVDT_true</t>
   </si>
   <si>
+    <t>SHMS HB Warm Return Valve</t>
+  </si>
+  <si>
+    <t>ecSQ1_vWR_LVDT_true</t>
+  </si>
+  <si>
+    <t>SHMS Q1 Warm Return Valve</t>
+  </si>
+  <si>
+    <t>ecSQ2_vWR_LVDT_true</t>
+  </si>
+  <si>
+    <t>SHMS Q2 Warm Return Valve</t>
+  </si>
+  <si>
+    <t>ecSQ3_vWR_LVDT_true</t>
+  </si>
+  <si>
     <t>SHMS Q3 Warm Return Valve</t>
-  </si>
-  <si>
-    <t>ecSQ1_vWR_LVDT_true</t>
-  </si>
-  <si>
-    <t>SHMS Q2 Warm Return Valve</t>
-  </si>
-  <si>
-    <t>ecSQ2_vWR_LVDT_true</t>
-  </si>
-  <si>
-    <t>SHMS Q1 Warm Return Valve</t>
-  </si>
-  <si>
-    <t>ecSQ3_vWR_LVDT_true</t>
-  </si>
-  <si>
-    <t>SHMS HB Warm Return Valve</t>
   </si>
   <si>
     <t>CEV6711C.ORBV</t>
@@ -1834,7 +1834,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1863,6 +1863,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1873,14 +1877,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1896,10 +1892,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1999,25 +1991,27 @@
   <dimension ref="A1:L304"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C145" activeCellId="0" sqref="C145"/>
+      <selection pane="bottomLeft" activeCell="D187" activeCellId="0" sqref="D187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.8163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
       <c r="L1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2054,18 +2048,18 @@
       <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="7"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
       <c r="L5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2109,7 +2103,7 @@
       <c r="L7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="0"/>
@@ -2129,10 +2123,10 @@
       <c r="D9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="7" t="n">
         <v>1.03</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="7" t="n">
         <v>1.08</v>
       </c>
       <c r="L9" s="3" t="s">
@@ -2152,10 +2146,10 @@
       <c r="D10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="7" t="n">
         <v>20</v>
       </c>
       <c r="L10" s="0"/>
@@ -2173,27 +2167,27 @@
       <c r="D11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="7" t="n">
         <v>-3</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="7" t="s">
         <v>31</v>
       </c>
       <c r="L11" s="0"/>
     </row>
-    <row r="12" s="9" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+    <row r="12" s="10" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="L12" s="11"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -2208,10 +2202,10 @@
       <c r="D13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1" t="n">
+      <c r="E13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="n">
         <v>20</v>
       </c>
       <c r="L13" s="0"/>
@@ -2229,10 +2223,10 @@
       <c r="D14" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="7" t="n">
         <v>3.9</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="7" t="n">
         <v>4.8</v>
       </c>
       <c r="L14" s="0"/>
@@ -2250,10 +2244,10 @@
       <c r="D15" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1" t="n">
+      <c r="E15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="n">
         <v>15</v>
       </c>
       <c r="L15" s="0"/>
@@ -2271,16 +2265,16 @@
       <c r="D16" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="F16" s="7" t="n">
         <v>10</v>
       </c>
       <c r="L16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -2292,10 +2286,10 @@
       <c r="D17" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1" t="n">
+      <c r="E17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="n">
         <v>10</v>
       </c>
       <c r="L17" s="0"/>
@@ -2313,10 +2307,10 @@
       <c r="D18" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L18" s="3" t="s">
@@ -2336,10 +2330,10 @@
       <c r="D19" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L19" s="3" t="s">
@@ -2359,10 +2353,10 @@
       <c r="D20" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L20" s="3" t="s">
@@ -2382,10 +2376,10 @@
       <c r="D21" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L21" s="3" t="s">
@@ -2405,10 +2399,10 @@
       <c r="D22" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L22" s="3" t="s">
@@ -2428,10 +2422,10 @@
       <c r="D23" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L23" s="3" t="s">
@@ -2451,10 +2445,10 @@
       <c r="D24" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L24" s="3" t="s">
@@ -2474,10 +2468,10 @@
       <c r="D25" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L25" s="3" t="s">
@@ -2497,10 +2491,10 @@
       <c r="D26" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L26" s="3" t="s">
@@ -2520,16 +2514,16 @@
       <c r="D27" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1" t="n">
+      <c r="E27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7" t="n">
         <v>20</v>
       </c>
       <c r="L27" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>82</v>
       </c>
       <c r="E29" s="0"/>
@@ -2546,10 +2540,10 @@
       <c r="D30" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="E30" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="F30" s="1" t="n">
+      <c r="F30" s="7" t="n">
         <v>18</v>
       </c>
       <c r="L30" s="3" t="s">
@@ -2566,10 +2560,10 @@
       <c r="D31" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="E31" s="7" t="n">
         <v>1.03</v>
       </c>
-      <c r="F31" s="1" t="n">
+      <c r="F31" s="7" t="n">
         <v>1.08</v>
       </c>
       <c r="L31" s="0"/>
@@ -2587,10 +2581,10 @@
       <c r="D32" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="E32" s="7" t="n">
         <v>2.8</v>
       </c>
-      <c r="F32" s="1" t="n">
+      <c r="F32" s="7" t="n">
         <v>3.2</v>
       </c>
       <c r="L32" s="3" t="s">
@@ -2610,10 +2604,10 @@
       <c r="D33" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="1" t="n">
+      <c r="E33" s="7" t="n">
         <v>1.05</v>
       </c>
-      <c r="F33" s="1" t="n">
+      <c r="F33" s="7" t="n">
         <v>1.15</v>
       </c>
       <c r="L33" s="0"/>
@@ -2665,10 +2659,10 @@
       <c r="D36" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="E36" s="1" t="n">
+      <c r="E36" s="7" t="n">
         <v>3.5</v>
       </c>
-      <c r="F36" s="1" t="n">
+      <c r="F36" s="7" t="n">
         <v>4</v>
       </c>
       <c r="L36" s="0"/>
@@ -2686,10 +2680,10 @@
       <c r="D37" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="E37" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F37" s="1" t="n">
+      <c r="F37" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L37" s="0"/>
@@ -2751,26 +2745,26 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" s="9" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
+    <row r="41" s="10" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="10" t="n">
+      <c r="E41" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="L41" s="11" t="s">
+      <c r="L41" s="2" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2804,10 +2798,10 @@
       <c r="D43" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="E43" s="1" t="n">
+      <c r="E43" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="F43" s="1" t="n">
+      <c r="F43" s="7" t="n">
         <v>15</v>
       </c>
       <c r="L43" s="3" t="s">
@@ -2844,10 +2838,10 @@
       <c r="D45" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="1" t="n">
+      <c r="E45" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="7" t="n">
         <v>20</v>
       </c>
       <c r="L45" s="3" t="s">
@@ -2860,24 +2854,41 @@
       <c r="L46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="0"/>
+      <c r="F47" s="0"/>
       <c r="L47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="0"/>
+      <c r="F48" s="0"/>
       <c r="L48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="0"/>
+      <c r="F49" s="0"/>
       <c r="L49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="0"/>
+      <c r="F50" s="0"/>
       <c r="L50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="0"/>
+      <c r="F51" s="0"/>
       <c r="L51" s="0"/>
     </row>
+    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="0"/>
+      <c r="F52" s="0"/>
+      <c r="L52" s="0"/>
+    </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="9" t="s">
         <v>132</v>
       </c>
+      <c r="E53" s="0"/>
+      <c r="F53" s="0"/>
       <c r="L53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2890,10 +2901,10 @@
       <c r="D54" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="E54" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" s="1" t="n">
+      <c r="E54" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="7" t="n">
         <v>100</v>
       </c>
       <c r="G54" s="0" t="n">
@@ -2913,10 +2924,10 @@
       <c r="D55" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="E55" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" s="1" t="n">
+      <c r="E55" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7" t="n">
         <v>100</v>
       </c>
       <c r="G55" s="0" t="n">
@@ -2936,10 +2947,10 @@
       <c r="D56" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="E56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" s="1" t="n">
+      <c r="E56" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="7" t="n">
         <v>100</v>
       </c>
       <c r="G56" s="0" t="n">
@@ -2959,10 +2970,10 @@
       <c r="D57" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E57" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" s="1" t="n">
+      <c r="E57" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="7" t="n">
         <v>100</v>
       </c>
       <c r="G57" s="0" t="n">
@@ -2982,10 +2993,10 @@
       <c r="D58" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="E58" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" s="1" t="n">
+      <c r="E58" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7" t="n">
         <v>100</v>
       </c>
       <c r="G58" s="0" t="n">
@@ -3005,10 +3016,10 @@
       <c r="D59" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="E59" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" s="1" t="n">
+      <c r="E59" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" s="7" t="n">
         <v>100</v>
       </c>
       <c r="G59" s="0" t="n">
@@ -3019,6 +3030,8 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="0"/>
+      <c r="F60" s="0"/>
       <c r="L60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,13 +3041,13 @@
       <c r="B61" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D61" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E61" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="1" t="n">
+      <c r="E61" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="7" t="n">
         <v>1722.3995</v>
       </c>
       <c r="L61" s="0"/>
@@ -3049,10 +3062,10 @@
       <c r="D62" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="E62" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F62" s="1" t="n">
+      <c r="E62" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L62" s="3" t="s">
@@ -3069,10 +3082,10 @@
       <c r="D63" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="E63" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F63" s="1" t="n">
+      <c r="E63" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L63" s="3" t="s">
@@ -3089,10 +3102,10 @@
       <c r="D64" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="E64" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F64" s="1" t="n">
+      <c r="E64" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" s="7" t="n">
         <v>1495.15332</v>
       </c>
       <c r="L64" s="0"/>
@@ -3107,10 +3120,10 @@
       <c r="D65" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="E65" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" s="1" t="n">
+      <c r="E65" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L65" s="3" t="s">
@@ -3127,10 +3140,10 @@
       <c r="D66" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="E66" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" s="1" t="n">
+      <c r="E66" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L66" s="3" t="s">
@@ -3147,10 +3160,10 @@
       <c r="D67" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E67" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F67" s="1" t="n">
+      <c r="E67" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" s="7" t="n">
         <v>1592.4747</v>
       </c>
       <c r="L67" s="0"/>
@@ -3165,10 +3178,10 @@
       <c r="D68" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E68" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F68" s="1" t="n">
+      <c r="E68" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L68" s="3" t="s">
@@ -3185,10 +3198,10 @@
       <c r="D69" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="E69" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F69" s="1" t="n">
+      <c r="E69" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L69" s="3" t="s">
@@ -3205,10 +3218,10 @@
       <c r="D70" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="E70" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F70" s="1" t="n">
+      <c r="E70" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" s="7" t="n">
         <v>1359.9608</v>
       </c>
       <c r="L70" s="0"/>
@@ -3223,10 +3236,10 @@
       <c r="D71" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="E71" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F71" s="1" t="n">
+      <c r="E71" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L71" s="3" t="s">
@@ -3243,10 +3256,10 @@
       <c r="D72" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="E72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F72" s="1" t="n">
+      <c r="E72" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L72" s="3" t="s">
@@ -3263,10 +3276,10 @@
       <c r="D73" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="E73" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F73" s="1" t="n">
+      <c r="E73" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" s="7" t="n">
         <v>1140</v>
       </c>
       <c r="L73" s="0"/>
@@ -3281,10 +3294,10 @@
       <c r="D74" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="E74" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F74" s="1" t="n">
+      <c r="E74" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L74" s="3" t="s">
@@ -3301,10 +3314,10 @@
       <c r="D75" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="E75" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F75" s="1" t="n">
+      <c r="E75" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L75" s="3" t="s">
@@ -3321,10 +3334,10 @@
       <c r="D76" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="E76" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F76" s="1" t="n">
+      <c r="E76" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" s="7" t="n">
         <v>1257.3917</v>
       </c>
       <c r="L76" s="0"/>
@@ -3339,10 +3352,10 @@
       <c r="D77" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="E77" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" s="1" t="n">
+      <c r="E77" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L77" s="3" t="s">
@@ -3359,10 +3372,10 @@
       <c r="D78" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="E78" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F78" s="1" t="n">
+      <c r="E78" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L78" s="3" t="s">
@@ -3379,9 +3392,10 @@
       <c r="D79" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="E79" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="E79" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" s="0"/>
       <c r="G79" s="0" t="n">
         <v>0</v>
       </c>
@@ -3400,10 +3414,10 @@
       <c r="D80" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="E80" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F80" s="1" t="n">
+      <c r="E80" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" s="7" t="n">
         <v>100</v>
       </c>
       <c r="G80" s="0" t="n">
@@ -3424,10 +3438,10 @@
       <c r="D81" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="E81" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F81" s="1" t="n">
+      <c r="E81" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" s="7" t="n">
         <v>100</v>
       </c>
       <c r="G81" s="0" t="n">
@@ -3436,10 +3450,12 @@
       <c r="L81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="0"/>
+      <c r="F82" s="0"/>
       <c r="L82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="13" t="s">
+      <c r="A83" s="12" t="s">
         <v>197</v>
       </c>
       <c r="B83" s="0" t="s">
@@ -3448,16 +3464,16 @@
       <c r="D83" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="E83" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F83" s="1" t="n">
+      <c r="E83" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L83" s="0"/>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="13" t="s">
+      <c r="A84" s="12" t="s">
         <v>199</v>
       </c>
       <c r="B84" s="0" t="s">
@@ -3466,16 +3482,16 @@
       <c r="D84" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="E84" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F84" s="1" t="n">
+      <c r="E84" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="12" t="s">
         <v>201</v>
       </c>
       <c r="B85" s="0" t="s">
@@ -3484,16 +3500,16 @@
       <c r="D85" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="E85" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F85" s="1" t="n">
+      <c r="E85" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L85" s="0"/>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="13" t="s">
+      <c r="A86" s="12" t="s">
         <v>203</v>
       </c>
       <c r="B86" s="0" t="s">
@@ -3502,16 +3518,16 @@
       <c r="D86" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="E86" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F86" s="1" t="n">
+      <c r="E86" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L86" s="0"/>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="13" t="s">
+      <c r="A87" s="12" t="s">
         <v>205</v>
       </c>
       <c r="B87" s="0" t="s">
@@ -3520,16 +3536,16 @@
       <c r="D87" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="E87" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F87" s="1" t="n">
+      <c r="E87" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L87" s="0"/>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="12" t="s">
         <v>207</v>
       </c>
       <c r="B88" s="0" t="s">
@@ -3538,16 +3554,16 @@
       <c r="D88" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="E88" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F88" s="1" t="n">
+      <c r="E88" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L88" s="0"/>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="13" t="s">
+      <c r="A89" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B89" s="0" t="s">
@@ -3556,16 +3572,16 @@
       <c r="D89" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E89" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F89" s="1" t="n">
+      <c r="E89" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L89" s="0"/>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="12" t="s">
         <v>211</v>
       </c>
       <c r="B90" s="0" t="s">
@@ -3574,10 +3590,10 @@
       <c r="D90" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="E90" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F90" s="1" t="n">
+      <c r="E90" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L90" s="3" t="s">
@@ -3585,7 +3601,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="13" t="s">
+      <c r="A91" s="12" t="s">
         <v>214</v>
       </c>
       <c r="B91" s="0" t="s">
@@ -3594,16 +3610,16 @@
       <c r="D91" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="E91" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F91" s="1" t="n">
+      <c r="E91" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="13" t="s">
+      <c r="A92" s="12" t="s">
         <v>216</v>
       </c>
       <c r="B92" s="0" t="s">
@@ -3612,16 +3628,16 @@
       <c r="D92" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="E92" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F92" s="1" t="n">
+      <c r="E92" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L92" s="0"/>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="13" t="s">
+      <c r="A93" s="12" t="s">
         <v>218</v>
       </c>
       <c r="B93" s="0" t="s">
@@ -3630,16 +3646,16 @@
       <c r="D93" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="E93" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F93" s="1" t="n">
+      <c r="E93" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L93" s="0"/>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="13" t="s">
+      <c r="A94" s="12" t="s">
         <v>220</v>
       </c>
       <c r="B94" s="0" t="s">
@@ -3648,16 +3664,16 @@
       <c r="D94" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="E94" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F94" s="1" t="n">
+      <c r="E94" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L94" s="0"/>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="13" t="s">
+      <c r="A95" s="12" t="s">
         <v>222</v>
       </c>
       <c r="B95" s="0" t="s">
@@ -3666,16 +3682,16 @@
       <c r="D95" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E95" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F95" s="1" t="n">
+      <c r="E95" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L95" s="0"/>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="13" t="s">
+      <c r="A96" s="12" t="s">
         <v>224</v>
       </c>
       <c r="B96" s="0" t="s">
@@ -3684,10 +3700,10 @@
       <c r="D96" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="E96" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F96" s="1" t="n">
+      <c r="E96" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F96" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L96" s="3" t="s">
@@ -3695,7 +3711,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="13" t="s">
+      <c r="A97" s="12" t="s">
         <v>226</v>
       </c>
       <c r="B97" s="0" t="s">
@@ -3704,16 +3720,16 @@
       <c r="D97" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E97" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F97" s="1" t="n">
+      <c r="E97" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F97" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="13" t="s">
+      <c r="A98" s="12" t="s">
         <v>228</v>
       </c>
       <c r="B98" s="0" t="s">
@@ -3722,16 +3738,16 @@
       <c r="D98" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="E98" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F98" s="1" t="n">
+      <c r="E98" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="13" t="s">
+      <c r="A99" s="12" t="s">
         <v>230</v>
       </c>
       <c r="B99" s="0" t="s">
@@ -3740,16 +3756,16 @@
       <c r="D99" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E99" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F99" s="1" t="n">
+      <c r="E99" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L99" s="0"/>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="13" t="s">
+      <c r="A100" s="12" t="s">
         <v>232</v>
       </c>
       <c r="B100" s="0" t="s">
@@ -3758,16 +3774,16 @@
       <c r="D100" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="E100" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F100" s="1" t="n">
+      <c r="E100" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L100" s="0"/>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="13" t="s">
+      <c r="A101" s="12" t="s">
         <v>234</v>
       </c>
       <c r="B101" s="0" t="s">
@@ -3776,16 +3792,16 @@
       <c r="D101" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E101" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F101" s="1" t="n">
+      <c r="E101" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L101" s="0"/>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="13" t="s">
+      <c r="A102" s="12" t="s">
         <v>236</v>
       </c>
       <c r="B102" s="0" t="s">
@@ -3794,10 +3810,10 @@
       <c r="D102" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="E102" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F102" s="1" t="n">
+      <c r="E102" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F102" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L102" s="3" t="s">
@@ -3805,16 +3821,28 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E103" s="0"/>
+      <c r="F103" s="0"/>
       <c r="L103" s="0"/>
     </row>
+    <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E104" s="0"/>
+      <c r="F104" s="0"/>
+      <c r="L104" s="0"/>
+    </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="8" t="s">
+      <c r="A105" s="9" t="s">
         <v>238</v>
       </c>
       <c r="E105" s="0"/>
       <c r="F105" s="0"/>
       <c r="L105" s="0"/>
     </row>
+    <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E106" s="0"/>
+      <c r="F106" s="0"/>
+      <c r="L106" s="0"/>
+    </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>239</v>
@@ -3828,6 +3856,8 @@
       <c r="D107" s="0" t="s">
         <v>241</v>
       </c>
+      <c r="E107" s="0"/>
+      <c r="F107" s="0"/>
       <c r="L107" s="0"/>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,6 +3873,8 @@
       <c r="D108" s="0" t="s">
         <v>244</v>
       </c>
+      <c r="E108" s="0"/>
+      <c r="F108" s="0"/>
       <c r="L108" s="0"/>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3858,10 +3890,10 @@
       <c r="D109" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="E109" s="1" t="n">
+      <c r="E109" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F109" s="1" t="n">
+      <c r="F109" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L109" s="0"/>
@@ -3879,10 +3911,10 @@
       <c r="D110" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="E110" s="1" t="n">
+      <c r="E110" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F110" s="1" t="n">
+      <c r="F110" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L110" s="3" t="s">
@@ -3902,10 +3934,10 @@
       <c r="D111" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="E111" s="1" t="n">
+      <c r="E111" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="F111" s="1" t="n">
+      <c r="F111" s="7" t="n">
         <v>90</v>
       </c>
       <c r="L111" s="0"/>
@@ -3923,10 +3955,10 @@
       <c r="D112" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="E112" s="1" t="n">
+      <c r="E112" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="F112" s="1" t="n">
+      <c r="F112" s="7" t="n">
         <v>90</v>
       </c>
       <c r="L112" s="3" t="s">
@@ -3946,10 +3978,10 @@
       <c r="D113" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E113" s="1" t="n">
+      <c r="E113" s="7" t="n">
         <v>-2416</v>
       </c>
-      <c r="F113" s="1" t="n">
+      <c r="F113" s="7" t="n">
         <v>2416</v>
       </c>
       <c r="L113" s="0"/>
@@ -3967,10 +3999,10 @@
       <c r="D114" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="E114" s="1" t="n">
+      <c r="E114" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F114" s="1" t="n">
+      <c r="F114" s="7" t="n">
         <v>70</v>
       </c>
       <c r="L114" s="0"/>
@@ -3988,16 +4020,16 @@
       <c r="D115" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E115" s="1" t="n">
+      <c r="E115" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F115" s="1" t="n">
+      <c r="F115" s="7" t="n">
         <v>70</v>
       </c>
       <c r="L115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="12" t="s">
+      <c r="A116" s="11" t="s">
         <v>266</v>
       </c>
       <c r="B116" s="0" t="s">
@@ -4009,16 +4041,16 @@
       <c r="D116" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="E116" s="1" t="n">
+      <c r="E116" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="F116" s="1" t="n">
+      <c r="F116" s="7" t="n">
         <v>58</v>
       </c>
       <c r="L116" s="0"/>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="12" t="s">
+      <c r="A117" s="11" t="s">
         <v>268</v>
       </c>
       <c r="B117" s="0" t="s">
@@ -4030,15 +4062,17 @@
       <c r="D117" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="E117" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F117" s="1" t="n">
+      <c r="E117" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L117" s="0"/>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E118" s="0"/>
+      <c r="F118" s="0"/>
       <c r="L118" s="0"/>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4054,6 +4088,8 @@
       <c r="D119" s="0" t="s">
         <v>273</v>
       </c>
+      <c r="E119" s="0"/>
+      <c r="F119" s="0"/>
       <c r="L119" s="0"/>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4069,6 +4105,8 @@
       <c r="D120" s="0" t="s">
         <v>276</v>
       </c>
+      <c r="E120" s="0"/>
+      <c r="F120" s="0"/>
       <c r="L120" s="0"/>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4084,10 +4122,10 @@
       <c r="D121" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="E121" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F121" s="1" t="n">
+      <c r="E121" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L121" s="0"/>
@@ -4105,10 +4143,10 @@
       <c r="D122" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="E122" s="1" t="n">
+      <c r="E122" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F122" s="1" t="n">
+      <c r="F122" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L122" s="0"/>
@@ -4126,10 +4164,10 @@
       <c r="D123" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="E123" s="1" t="n">
+      <c r="E123" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F123" s="1" t="n">
+      <c r="F123" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L123" s="3" t="s">
@@ -4149,10 +4187,10 @@
       <c r="D124" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="E124" s="1" t="n">
+      <c r="E124" s="7" t="n">
         <v>-3770</v>
       </c>
-      <c r="F124" s="1" t="n">
+      <c r="F124" s="7" t="n">
         <v>3770</v>
       </c>
       <c r="L124" s="0"/>
@@ -4170,10 +4208,10 @@
       <c r="D125" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E125" s="1" t="n">
+      <c r="E125" s="7" t="n">
         <v>88</v>
       </c>
-      <c r="F125" s="1" t="n">
+      <c r="F125" s="7" t="n">
         <v>111</v>
       </c>
       <c r="L125" s="0"/>
@@ -4191,10 +4229,10 @@
       <c r="D126" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="E126" s="1" t="n">
+      <c r="E126" s="7" t="n">
         <v>88</v>
       </c>
-      <c r="F126" s="1" t="n">
+      <c r="F126" s="7" t="n">
         <v>111</v>
       </c>
       <c r="L126" s="0"/>
@@ -4212,10 +4250,10 @@
       <c r="D127" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="E127" s="1" t="n">
+      <c r="E127" s="7" t="n">
         <v>45</v>
       </c>
-      <c r="F127" s="1" t="n">
+      <c r="F127" s="7" t="n">
         <v>65</v>
       </c>
       <c r="L127" s="0"/>
@@ -4233,13 +4271,18 @@
       <c r="D128" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="E128" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F128" s="1" t="n">
+      <c r="E128" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F128" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L128" s="0"/>
+    </row>
+    <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E129" s="0"/>
+      <c r="F129" s="0"/>
+      <c r="L129" s="0"/>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
@@ -4254,10 +4297,10 @@
       <c r="D130" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="E130" s="1" t="n">
+      <c r="E130" s="7" t="n">
         <v>55</v>
       </c>
-      <c r="F130" s="1" t="n">
+      <c r="F130" s="7" t="n">
         <v>65</v>
       </c>
       <c r="L130" s="0"/>
@@ -4272,10 +4315,10 @@
       <c r="D131" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="E131" s="1" t="n">
+      <c r="E131" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F131" s="1" t="n">
+      <c r="F131" s="7" t="n">
         <v>50</v>
       </c>
       <c r="L131" s="0"/>
@@ -4290,10 +4333,10 @@
       <c r="D132" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="E132" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F132" s="1" t="n">
+      <c r="E132" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" s="7" t="n">
         <v>2</v>
       </c>
       <c r="L132" s="0"/>
@@ -4311,10 +4354,10 @@
       <c r="D133" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="E133" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F133" s="1" t="n">
+      <c r="E133" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F133" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L133" s="3" t="s">
@@ -4334,10 +4377,10 @@
       <c r="D134" s="0" t="s">
         <v>314</v>
       </c>
-      <c r="E134" s="1" t="n">
+      <c r="E134" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F134" s="1" t="n">
+      <c r="F134" s="7" t="n">
         <v>1300</v>
       </c>
       <c r="L134" s="3" t="s">
@@ -4357,22 +4400,29 @@
       <c r="D135" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="E135" s="1" t="n">
+      <c r="E135" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F135" s="1" t="n">
+      <c r="F135" s="7" t="n">
         <v>300</v>
       </c>
       <c r="L135" s="0"/>
     </row>
+    <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E136" s="0"/>
+      <c r="F136" s="0"/>
+      <c r="L136" s="0"/>
+    </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="8" t="s">
+      <c r="A137" s="9" t="s">
         <v>319</v>
       </c>
+      <c r="E137" s="0"/>
+      <c r="F137" s="0"/>
       <c r="L137" s="0"/>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="12" t="s">
+      <c r="A138" s="11" t="s">
         <v>320</v>
       </c>
       <c r="B138" s="0" t="s">
@@ -4381,16 +4431,16 @@
       <c r="D138" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="E138" s="1" t="n">
+      <c r="E138" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F138" s="1" t="n">
+      <c r="F138" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="12" t="s">
+      <c r="A139" s="11" t="s">
         <v>322</v>
       </c>
       <c r="B139" s="0" t="s">
@@ -4399,16 +4449,16 @@
       <c r="D139" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="E139" s="1" t="n">
+      <c r="E139" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F139" s="1" t="n">
+      <c r="F139" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L139" s="0"/>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="12" t="s">
+      <c r="A140" s="11" t="s">
         <v>324</v>
       </c>
       <c r="B140" s="0" t="s">
@@ -4417,16 +4467,16 @@
       <c r="D140" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="E140" s="1" t="n">
+      <c r="E140" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F140" s="1" t="n">
+      <c r="F140" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L140" s="0"/>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="12" t="s">
+      <c r="A141" s="11" t="s">
         <v>326</v>
       </c>
       <c r="B141" s="0" t="s">
@@ -4435,16 +4485,16 @@
       <c r="D141" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="E141" s="1" t="n">
+      <c r="E141" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F141" s="1" t="n">
+      <c r="F141" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L141" s="0"/>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="12" t="s">
+      <c r="A142" s="11" t="s">
         <v>328</v>
       </c>
       <c r="B142" s="0" t="s">
@@ -4453,16 +4503,16 @@
       <c r="D142" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="E142" s="1" t="n">
+      <c r="E142" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F142" s="1" t="n">
+      <c r="F142" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L142" s="0"/>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="12" t="s">
+      <c r="A143" s="11" t="s">
         <v>330</v>
       </c>
       <c r="B143" s="0" t="s">
@@ -4471,16 +4521,16 @@
       <c r="D143" s="0" t="s">
         <v>331</v>
       </c>
-      <c r="E143" s="1" t="n">
+      <c r="E143" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F143" s="1" t="n">
+      <c r="F143" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L143" s="0"/>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="12" t="s">
+      <c r="A144" s="11" t="s">
         <v>332</v>
       </c>
       <c r="B144" s="0" t="s">
@@ -4489,16 +4539,16 @@
       <c r="D144" s="0" t="s">
         <v>333</v>
       </c>
-      <c r="E144" s="1" t="n">
+      <c r="E144" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F144" s="1" t="n">
+      <c r="F144" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L144" s="0"/>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="12" t="s">
+      <c r="A145" s="11" t="s">
         <v>334</v>
       </c>
       <c r="B145" s="0" t="s">
@@ -4507,16 +4557,16 @@
       <c r="D145" s="0" t="s">
         <v>335</v>
       </c>
-      <c r="E145" s="1" t="n">
+      <c r="E145" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F145" s="1" t="n">
+      <c r="F145" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L145" s="0"/>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="12" t="s">
+      <c r="A146" s="11" t="s">
         <v>336</v>
       </c>
       <c r="B146" s="0" t="s">
@@ -4525,10 +4575,10 @@
       <c r="D146" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="E146" s="1" t="n">
+      <c r="E146" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F146" s="1" t="n">
+      <c r="F146" s="7" t="n">
         <v>80</v>
       </c>
       <c r="L146" s="0"/>
@@ -4543,10 +4593,10 @@
       <c r="D147" s="0" t="s">
         <v>339</v>
       </c>
-      <c r="E147" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F147" s="1" t="n">
+      <c r="E147" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F147" s="7" t="n">
         <v>1100</v>
       </c>
       <c r="L147" s="0"/>
@@ -4561,10 +4611,10 @@
       <c r="D148" s="0" t="s">
         <v>341</v>
       </c>
-      <c r="E148" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F148" s="1" t="n">
+      <c r="E148" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F148" s="7" t="n">
         <v>1100</v>
       </c>
       <c r="L148" s="0"/>
@@ -4579,10 +4629,10 @@
       <c r="D149" s="0" t="s">
         <v>343</v>
       </c>
-      <c r="E149" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F149" s="1" t="n">
+      <c r="E149" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F149" s="7" t="n">
         <v>1100</v>
       </c>
       <c r="L149" s="0"/>
@@ -4597,10 +4647,10 @@
       <c r="D150" s="0" t="s">
         <v>345</v>
       </c>
-      <c r="E150" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F150" s="1" t="n">
+      <c r="E150" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F150" s="7" t="n">
         <v>3000</v>
       </c>
       <c r="L150" s="0"/>
@@ -4615,10 +4665,10 @@
       <c r="D151" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="E151" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F151" s="1" t="n">
+      <c r="E151" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F151" s="7" t="n">
         <v>3950</v>
       </c>
       <c r="L151" s="0"/>
@@ -4633,10 +4683,10 @@
       <c r="D152" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="E152" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F152" s="1" t="n">
+      <c r="E152" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F152" s="7" t="n">
         <v>3500</v>
       </c>
       <c r="L152" s="0"/>
@@ -4651,10 +4701,10 @@
       <c r="D153" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="E153" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F153" s="1" t="n">
+      <c r="E153" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F153" s="7" t="n">
         <v>3660</v>
       </c>
       <c r="L153" s="0"/>
@@ -4669,10 +4719,10 @@
       <c r="D154" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="E154" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F154" s="1" t="n">
+      <c r="E154" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F154" s="7" t="n">
         <v>2500</v>
       </c>
       <c r="L154" s="0"/>
@@ -4687,10 +4737,10 @@
       <c r="D155" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="E155" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F155" s="1" t="n">
+      <c r="E155" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F155" s="7" t="n">
         <v>3450</v>
       </c>
       <c r="L155" s="0"/>
@@ -4705,10 +4755,10 @@
       <c r="D156" s="0" t="s">
         <v>358</v>
       </c>
-      <c r="E156" s="1" t="n">
+      <c r="E156" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F156" s="1" t="n">
+      <c r="F156" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L156" s="3" t="s">
@@ -4725,10 +4775,10 @@
       <c r="D157" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="E157" s="1" t="n">
+      <c r="E157" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F157" s="1" t="n">
+      <c r="F157" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L157" s="3" t="s">
@@ -4745,10 +4795,10 @@
       <c r="D158" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="E158" s="1" t="n">
+      <c r="E158" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F158" s="1" t="n">
+      <c r="F158" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L158" s="3" t="s">
@@ -4765,10 +4815,10 @@
       <c r="D159" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="E159" s="1" t="n">
+      <c r="E159" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F159" s="1" t="n">
+      <c r="F159" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L159" s="3" t="s">
@@ -4785,10 +4835,10 @@
       <c r="D160" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="E160" s="1" t="n">
+      <c r="E160" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F160" s="1" t="n">
+      <c r="F160" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L160" s="3" t="s">
@@ -4805,10 +4855,10 @@
       <c r="D161" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="E161" s="1" t="n">
+      <c r="E161" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F161" s="1" t="n">
+      <c r="F161" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L161" s="3" t="s">
@@ -4825,10 +4875,10 @@
       <c r="D162" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="E162" s="1" t="n">
+      <c r="E162" s="7" t="n">
         <v>3300</v>
       </c>
-      <c r="F162" s="1" t="n">
+      <c r="F162" s="7" t="n">
         <v>7500</v>
       </c>
       <c r="L162" s="3" t="s">
@@ -4845,10 +4895,10 @@
       <c r="D163" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="E163" s="1" t="n">
+      <c r="E163" s="7" t="n">
         <v>3300</v>
       </c>
-      <c r="F163" s="1" t="n">
+      <c r="F163" s="7" t="n">
         <v>7500</v>
       </c>
       <c r="L163" s="3" t="s">
@@ -4865,10 +4915,10 @@
       <c r="D164" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="E164" s="1" t="n">
+      <c r="E164" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F164" s="1" t="n">
+      <c r="F164" s="7" t="n">
         <v>110</v>
       </c>
       <c r="L164" s="3" t="s">
@@ -4885,10 +4935,10 @@
       <c r="D165" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="E165" s="1" t="n">
+      <c r="E165" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F165" s="1" t="n">
+      <c r="F165" s="7" t="n">
         <v>110</v>
       </c>
       <c r="L165" s="3" t="s">
@@ -4905,10 +4955,10 @@
       <c r="D166" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="E166" s="1" t="n">
+      <c r="E166" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F166" s="1" t="n">
+      <c r="F166" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L166" s="3" t="s">
@@ -4925,10 +4975,10 @@
       <c r="D167" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="E167" s="1" t="n">
+      <c r="E167" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F167" s="1" t="n">
+      <c r="F167" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L167" s="3" t="s">
@@ -4945,10 +4995,10 @@
       <c r="D168" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="E168" s="1" t="n">
+      <c r="E168" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F168" s="1" t="n">
+      <c r="F168" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L168" s="3" t="s">
@@ -4965,10 +5015,10 @@
       <c r="D169" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="E169" s="1" t="n">
+      <c r="E169" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F169" s="1" t="n">
+      <c r="F169" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L169" s="3" t="s">
@@ -4985,10 +5035,10 @@
       <c r="D170" s="0" t="s">
         <v>388</v>
       </c>
-      <c r="E170" s="1" t="n">
+      <c r="E170" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F170" s="1" t="n">
+      <c r="F170" s="7" t="n">
         <v>90</v>
       </c>
       <c r="L170" s="3" t="s">
@@ -5005,10 +5055,10 @@
       <c r="D171" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="E171" s="1" t="n">
+      <c r="E171" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F171" s="1" t="n">
+      <c r="F171" s="7" t="n">
         <v>90</v>
       </c>
       <c r="L171" s="3" t="s">
@@ -5025,10 +5075,10 @@
       <c r="D172" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="E172" s="1" t="n">
+      <c r="E172" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F172" s="1" t="n">
+      <c r="F172" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L172" s="3" t="s">
@@ -5045,10 +5095,10 @@
       <c r="D173" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="E173" s="1" t="n">
+      <c r="E173" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F173" s="1" t="n">
+      <c r="F173" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L173" s="3" t="s">
@@ -5056,15 +5106,19 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E174" s="0"/>
+      <c r="F174" s="0"/>
       <c r="L174" s="0"/>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="12" t="s">
+      <c r="A175" s="11" t="s">
         <v>395</v>
       </c>
       <c r="D175" s="0" t="s">
         <v>396</v>
       </c>
+      <c r="E175" s="0"/>
+      <c r="F175" s="0"/>
       <c r="L175" s="0"/>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5074,6 +5128,8 @@
       <c r="D176" s="0" t="s">
         <v>398</v>
       </c>
+      <c r="E176" s="0"/>
+      <c r="F176" s="0"/>
       <c r="L176" s="0"/>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5083,6 +5139,8 @@
       <c r="D177" s="0" t="s">
         <v>400</v>
       </c>
+      <c r="E177" s="0"/>
+      <c r="F177" s="0"/>
       <c r="L177" s="0"/>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5092,18 +5150,24 @@
       <c r="D178" s="0" t="s">
         <v>402</v>
       </c>
+      <c r="E178" s="0"/>
+      <c r="F178" s="0"/>
       <c r="L178" s="0"/>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E179" s="0"/>
+      <c r="F179" s="0"/>
       <c r="L179" s="0"/>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="12" t="s">
+      <c r="A180" s="11" t="s">
         <v>403</v>
       </c>
       <c r="D180" s="0" t="s">
         <v>404</v>
       </c>
+      <c r="E180" s="0"/>
+      <c r="F180" s="0"/>
       <c r="L180" s="0"/>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5113,6 +5177,8 @@
       <c r="D181" s="0" t="s">
         <v>406</v>
       </c>
+      <c r="E181" s="0"/>
+      <c r="F181" s="0"/>
       <c r="L181" s="0"/>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5122,6 +5188,8 @@
       <c r="D182" s="0" t="s">
         <v>408</v>
       </c>
+      <c r="E182" s="0"/>
+      <c r="F182" s="0"/>
       <c r="L182" s="0"/>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5131,144 +5199,182 @@
       <c r="D183" s="0" t="s">
         <v>410</v>
       </c>
+      <c r="E183" s="0"/>
+      <c r="F183" s="0"/>
       <c r="L183" s="0"/>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E184" s="0"/>
+      <c r="F184" s="0"/>
       <c r="L184" s="0"/>
     </row>
-    <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>411</v>
       </c>
       <c r="D185" s="0" t="s">
         <v>412</v>
       </c>
+      <c r="E185" s="0"/>
+      <c r="F185" s="0"/>
       <c r="L185" s="0"/>
     </row>
-    <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>413</v>
       </c>
       <c r="D186" s="0" t="s">
         <v>414</v>
       </c>
+      <c r="E186" s="0"/>
+      <c r="F186" s="0"/>
       <c r="L186" s="0"/>
     </row>
-    <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
         <v>415</v>
       </c>
       <c r="D187" s="0" t="s">
         <v>416</v>
       </c>
+      <c r="E187" s="0"/>
+      <c r="F187" s="0"/>
       <c r="L187" s="0"/>
     </row>
-    <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
         <v>417</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>418</v>
       </c>
+      <c r="E188" s="0"/>
+      <c r="F188" s="0"/>
       <c r="L188" s="0"/>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E189" s="0"/>
+      <c r="F189" s="0"/>
       <c r="L189" s="0"/>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="12" t="s">
+      <c r="A190" s="11" t="s">
         <v>419</v>
       </c>
       <c r="D190" s="0" t="s">
         <v>420</v>
       </c>
+      <c r="E190" s="0"/>
+      <c r="F190" s="0"/>
       <c r="L190" s="0"/>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="12" t="s">
+      <c r="A191" s="11" t="s">
         <v>421</v>
       </c>
       <c r="D191" s="0" t="s">
         <v>422</v>
       </c>
+      <c r="E191" s="0"/>
+      <c r="F191" s="0"/>
       <c r="L191" s="0"/>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="12" t="s">
+      <c r="A192" s="11" t="s">
         <v>423</v>
       </c>
       <c r="D192" s="0" t="s">
         <v>424</v>
       </c>
+      <c r="E192" s="0"/>
+      <c r="F192" s="0"/>
       <c r="L192" s="0"/>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="12" t="s">
+      <c r="A193" s="11" t="s">
         <v>425</v>
       </c>
       <c r="D193" s="0" t="s">
         <v>426</v>
       </c>
+      <c r="E193" s="0"/>
+      <c r="F193" s="0"/>
       <c r="L193" s="0"/>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="12" t="s">
+      <c r="A194" s="11" t="s">
         <v>427</v>
       </c>
       <c r="D194" s="0" t="s">
         <v>428</v>
       </c>
+      <c r="E194" s="0"/>
+      <c r="F194" s="0"/>
       <c r="L194" s="0"/>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E195" s="0"/>
+      <c r="F195" s="0"/>
       <c r="L195" s="0"/>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="12" t="s">
+      <c r="A196" s="11" t="s">
         <v>429</v>
       </c>
       <c r="D196" s="0" t="s">
         <v>430</v>
       </c>
+      <c r="E196" s="0"/>
+      <c r="F196" s="0"/>
       <c r="L196" s="0"/>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="12" t="s">
+      <c r="A197" s="11" t="s">
         <v>431</v>
       </c>
       <c r="D197" s="0" t="s">
         <v>432</v>
       </c>
+      <c r="E197" s="0"/>
+      <c r="F197" s="0"/>
       <c r="L197" s="0"/>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="12" t="s">
+      <c r="A198" s="11" t="s">
         <v>433</v>
       </c>
       <c r="D198" s="0" t="s">
         <v>434</v>
       </c>
+      <c r="E198" s="0"/>
+      <c r="F198" s="0"/>
       <c r="L198" s="0"/>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="12" t="s">
+      <c r="A199" s="11" t="s">
         <v>435</v>
       </c>
       <c r="D199" s="0" t="s">
         <v>436</v>
       </c>
+      <c r="E199" s="0"/>
+      <c r="F199" s="0"/>
       <c r="L199" s="0"/>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="12" t="s">
+      <c r="A200" s="11" t="s">
         <v>437</v>
       </c>
       <c r="D200" s="0" t="s">
         <v>438</v>
       </c>
+      <c r="E200" s="0"/>
+      <c r="F200" s="0"/>
       <c r="L200" s="0"/>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E201" s="0"/>
+      <c r="F201" s="0"/>
       <c r="L201" s="0"/>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5278,82 +5384,116 @@
       <c r="D202" s="0" t="s">
         <v>440</v>
       </c>
+      <c r="E202" s="0"/>
+      <c r="F202" s="0"/>
       <c r="L202" s="0"/>
     </row>
-    <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
         <v>441</v>
       </c>
       <c r="D203" s="0" t="s">
         <v>442</v>
       </c>
+      <c r="E203" s="0"/>
+      <c r="F203" s="0"/>
       <c r="L203" s="0"/>
     </row>
-    <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
         <v>443</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>444</v>
       </c>
+      <c r="E204" s="0"/>
+      <c r="F204" s="0"/>
       <c r="L204" s="0"/>
     </row>
-    <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
         <v>445</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>446</v>
       </c>
+      <c r="E205" s="0"/>
+      <c r="F205" s="0"/>
       <c r="L205" s="0"/>
     </row>
-    <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
         <v>447</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>448</v>
       </c>
+      <c r="E206" s="0"/>
+      <c r="F206" s="0"/>
       <c r="L206" s="0"/>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E207" s="0"/>
+      <c r="F207" s="0"/>
       <c r="L207" s="0"/>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E208" s="0"/>
+      <c r="F208" s="0"/>
       <c r="L208" s="0"/>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E209" s="0"/>
+      <c r="F209" s="0"/>
       <c r="L209" s="0"/>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E210" s="0"/>
+      <c r="F210" s="0"/>
       <c r="L210" s="0"/>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E211" s="0"/>
+      <c r="F211" s="0"/>
       <c r="L211" s="0"/>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E212" s="0"/>
+      <c r="F212" s="0"/>
       <c r="L212" s="0"/>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E213" s="0"/>
+      <c r="F213" s="0"/>
       <c r="L213" s="0"/>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E214" s="0"/>
+      <c r="F214" s="0"/>
       <c r="L214" s="0"/>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E215" s="0"/>
+      <c r="F215" s="0"/>
       <c r="L215" s="0"/>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E216" s="0"/>
+      <c r="F216" s="0"/>
       <c r="L216" s="0"/>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E217" s="0"/>
+      <c r="F217" s="0"/>
       <c r="L217" s="0"/>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E218" s="0"/>
+      <c r="F218" s="0"/>
       <c r="L218" s="0"/>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="12" t="s">
+      <c r="A219" s="11" t="s">
         <v>449</v>
       </c>
       <c r="B219" s="0" t="s">
@@ -5362,10 +5502,10 @@
       <c r="D219" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="E219" s="1" t="n">
+      <c r="E219" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F219" s="1" t="n">
+      <c r="F219" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L219" s="0"/>
@@ -5380,10 +5520,10 @@
       <c r="D220" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="E220" s="1" t="n">
+      <c r="E220" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F220" s="1" t="n">
+      <c r="F220" s="7" t="n">
         <v>100</v>
       </c>
       <c r="L220" s="0"/>
@@ -5398,6 +5538,8 @@
       <c r="D221" s="0" t="s">
         <v>454</v>
       </c>
+      <c r="E221" s="0"/>
+      <c r="F221" s="0"/>
       <c r="L221" s="3" t="s">
         <v>455</v>
       </c>
@@ -5412,15 +5554,17 @@
       <c r="D222" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="E222" s="1" t="n">
+      <c r="E222" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F222" s="1" t="n">
+      <c r="F222" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L222" s="0"/>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E223" s="0"/>
+      <c r="F223" s="0"/>
       <c r="L223" s="0"/>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5433,10 +5577,10 @@
       <c r="D224" s="0" t="s">
         <v>458</v>
       </c>
-      <c r="E224" s="1" t="n">
+      <c r="E224" s="7" t="n">
         <v>5.1</v>
       </c>
-      <c r="F224" s="1" t="n">
+      <c r="F224" s="7" t="n">
         <v>5.3</v>
       </c>
       <c r="L224" s="0"/>
@@ -5451,10 +5595,10 @@
       <c r="D225" s="0" t="s">
         <v>460</v>
       </c>
-      <c r="E225" s="1" t="n">
+      <c r="E225" s="7" t="n">
         <v>5.2</v>
       </c>
-      <c r="F225" s="1" t="n">
+      <c r="F225" s="7" t="n">
         <v>5.4</v>
       </c>
       <c r="L225" s="0"/>
@@ -5469,10 +5613,10 @@
       <c r="D226" s="0" t="s">
         <v>462</v>
       </c>
-      <c r="E226" s="1" t="n">
+      <c r="E226" s="7" t="n">
         <v>5.5</v>
       </c>
-      <c r="F226" s="1" t="n">
+      <c r="F226" s="7" t="n">
         <v>6.5</v>
       </c>
       <c r="L226" s="0"/>
@@ -5487,10 +5631,10 @@
       <c r="D227" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="E227" s="1" t="n">
+      <c r="E227" s="7" t="n">
         <v>5.1</v>
       </c>
-      <c r="F227" s="1" t="n">
+      <c r="F227" s="7" t="n">
         <v>5.3</v>
       </c>
       <c r="L227" s="0"/>
@@ -5499,12 +5643,16 @@
       <c r="A228" s="0" t="s">
         <v>465</v>
       </c>
+      <c r="E228" s="0"/>
+      <c r="F228" s="0"/>
       <c r="L228" s="0"/>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
         <v>466</v>
       </c>
+      <c r="E229" s="0"/>
+      <c r="F229" s="0"/>
       <c r="L229" s="0"/>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5517,6 +5665,8 @@
       <c r="D230" s="0" t="s">
         <v>468</v>
       </c>
+      <c r="E230" s="0"/>
+      <c r="F230" s="0"/>
       <c r="L230" s="0"/>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5529,6 +5679,8 @@
       <c r="D231" s="0" t="s">
         <v>470</v>
       </c>
+      <c r="E231" s="0"/>
+      <c r="F231" s="0"/>
       <c r="L231" s="0"/>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5541,6 +5693,8 @@
       <c r="D232" s="0" t="s">
         <v>472</v>
       </c>
+      <c r="E232" s="0"/>
+      <c r="F232" s="0"/>
       <c r="L232" s="0"/>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5553,6 +5707,8 @@
       <c r="D233" s="0" t="s">
         <v>474</v>
       </c>
+      <c r="E233" s="0"/>
+      <c r="F233" s="0"/>
       <c r="L233" s="0"/>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5565,6 +5721,8 @@
       <c r="D234" s="0" t="s">
         <v>477</v>
       </c>
+      <c r="E234" s="0"/>
+      <c r="F234" s="0"/>
       <c r="L234" s="0"/>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5577,30 +5735,67 @@
       <c r="D235" s="0" t="s">
         <v>479</v>
       </c>
+      <c r="E235" s="0"/>
+      <c r="F235" s="0"/>
       <c r="L235" s="0"/>
     </row>
+    <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E236" s="0"/>
+      <c r="F236" s="0"/>
+      <c r="L236" s="0"/>
+    </row>
+    <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E237" s="0"/>
+      <c r="F237" s="0"/>
+      <c r="L237" s="0"/>
+    </row>
+    <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E238" s="0"/>
+      <c r="F238" s="0"/>
+      <c r="L238" s="0"/>
+    </row>
+    <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E239" s="0"/>
+      <c r="F239" s="0"/>
+      <c r="L239" s="0"/>
+    </row>
+    <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E240" s="0"/>
+      <c r="F240" s="0"/>
+      <c r="L240" s="0"/>
+    </row>
+    <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E241" s="0"/>
+      <c r="F241" s="0"/>
+      <c r="L241" s="0"/>
+    </row>
+    <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E242" s="0"/>
+      <c r="F242" s="0"/>
+      <c r="L242" s="0"/>
+    </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="14" t="s">
+      <c r="A243" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="B243" s="15"/>
-      <c r="C243" s="15"/>
-      <c r="D243" s="15"/>
+      <c r="B243" s="14"/>
+      <c r="C243" s="14"/>
+      <c r="D243" s="14"/>
       <c r="E243" s="0"/>
       <c r="F243" s="0"/>
       <c r="L243" s="0"/>
     </row>
     <row r="244" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="16" t="s">
+      <c r="A244" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B244" s="16"/>
-      <c r="C244" s="16"/>
-      <c r="D244" s="16"/>
-      <c r="E244" s="17" t="s">
+      <c r="B244" s="10"/>
+      <c r="C244" s="10"/>
+      <c r="D244" s="10"/>
+      <c r="E244" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F244" s="17" t="s">
+      <c r="F244" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G244" s="3" t="s">
@@ -5722,6 +5917,11 @@
         <v>496</v>
       </c>
     </row>
+    <row r="250" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E250" s="0"/>
+      <c r="F250" s="0"/>
+      <c r="L250" s="0"/>
+    </row>
     <row r="251" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
         <v>497</v>
@@ -5822,6 +6022,11 @@
         <v>496</v>
       </c>
     </row>
+    <row r="256" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E256" s="0"/>
+      <c r="F256" s="0"/>
+      <c r="L256" s="0"/>
+    </row>
     <row r="257" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
         <v>508</v>
@@ -5921,6 +6126,11 @@
       <c r="L261" s="3" t="s">
         <v>496</v>
       </c>
+    </row>
+    <row r="262" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E262" s="0"/>
+      <c r="F262" s="0"/>
+      <c r="L262" s="0"/>
     </row>
     <row r="263" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
@@ -6048,28 +6258,38 @@
       <c r="F269" s="0"/>
       <c r="L269" s="0"/>
     </row>
+    <row r="270" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E270" s="0"/>
+      <c r="F270" s="0"/>
+      <c r="L270" s="0"/>
+    </row>
+    <row r="271" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E271" s="0"/>
+      <c r="F271" s="0"/>
+      <c r="L271" s="0"/>
+    </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="18" t="s">
+      <c r="A272" s="16" t="s">
         <v>536</v>
       </c>
-      <c r="B272" s="19"/>
-      <c r="C272" s="19"/>
-      <c r="D272" s="19"/>
+      <c r="B272" s="17"/>
+      <c r="C272" s="17"/>
+      <c r="D272" s="17"/>
       <c r="E272" s="0"/>
       <c r="F272" s="0"/>
       <c r="L272" s="0"/>
     </row>
     <row r="273" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="16" t="s">
+      <c r="A273" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B273" s="16"/>
-      <c r="C273" s="16"/>
-      <c r="D273" s="16"/>
-      <c r="E273" s="17" t="s">
+      <c r="B273" s="10"/>
+      <c r="C273" s="10"/>
+      <c r="D273" s="10"/>
+      <c r="E273" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F273" s="17" t="s">
+      <c r="F273" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G273" s="3" t="s">
@@ -6101,10 +6321,10 @@
       <c r="D274" s="0" t="s">
         <v>483</v>
       </c>
-      <c r="E274" s="1" t="n">
+      <c r="E274" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="F274" s="1" t="n">
+      <c r="F274" s="7" t="n">
         <v>50</v>
       </c>
       <c r="L274" s="3" t="s">
@@ -6121,10 +6341,10 @@
       <c r="D275" s="0" t="s">
         <v>486</v>
       </c>
-      <c r="E275" s="1" t="n">
+      <c r="E275" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="F275" s="1" t="n">
+      <c r="F275" s="7" t="n">
         <v>24</v>
       </c>
       <c r="L275" s="3" t="s">
@@ -6141,10 +6361,10 @@
       <c r="D276" s="0" t="s">
         <v>490</v>
       </c>
-      <c r="E276" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F276" s="1" t="n">
+      <c r="E276" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F276" s="7" t="n">
         <v>500</v>
       </c>
       <c r="L276" s="3" t="s">
@@ -6161,10 +6381,10 @@
       <c r="D277" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="E277" s="1" t="n">
+      <c r="E277" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="F277" s="1" t="n">
+      <c r="F277" s="7" t="n">
         <v>16</v>
       </c>
       <c r="L277" s="3" t="s">
@@ -6181,10 +6401,10 @@
       <c r="D278" s="0" t="s">
         <v>495</v>
       </c>
-      <c r="E278" s="1" t="n">
+      <c r="E278" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="F278" s="1" t="n">
+      <c r="F278" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L278" s="3" t="s">
@@ -6192,6 +6412,8 @@
       </c>
     </row>
     <row r="279" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E279" s="0"/>
+      <c r="F279" s="0"/>
       <c r="L279" s="0"/>
     </row>
     <row r="280" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6204,10 +6426,10 @@
       <c r="D280" s="0" t="s">
         <v>498</v>
       </c>
-      <c r="E280" s="1" t="n">
+      <c r="E280" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="F280" s="1" t="n">
+      <c r="F280" s="7" t="n">
         <v>50</v>
       </c>
       <c r="L280" s="3" t="s">
@@ -6224,10 +6446,10 @@
       <c r="D281" s="0" t="s">
         <v>501</v>
       </c>
-      <c r="E281" s="1" t="n">
+      <c r="E281" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="F281" s="1" t="n">
+      <c r="F281" s="7" t="n">
         <v>24</v>
       </c>
       <c r="L281" s="3" t="s">
@@ -6244,10 +6466,10 @@
       <c r="D282" s="0" t="s">
         <v>503</v>
       </c>
-      <c r="E282" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F282" s="1" t="n">
+      <c r="E282" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F282" s="7" t="n">
         <v>500</v>
       </c>
       <c r="L282" s="3" t="s">
@@ -6264,10 +6486,10 @@
       <c r="D283" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="E283" s="1" t="n">
+      <c r="E283" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="F283" s="1" t="n">
+      <c r="F283" s="7" t="n">
         <v>16</v>
       </c>
       <c r="L283" s="3" t="s">
@@ -6284,10 +6506,10 @@
       <c r="D284" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="E284" s="1" t="n">
+      <c r="E284" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="F284" s="1" t="n">
+      <c r="F284" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L284" s="3" t="s">
@@ -6295,6 +6517,8 @@
       </c>
     </row>
     <row r="285" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E285" s="0"/>
+      <c r="F285" s="0"/>
       <c r="L285" s="0"/>
     </row>
     <row r="286" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6307,10 +6531,10 @@
       <c r="D286" s="0" t="s">
         <v>509</v>
       </c>
-      <c r="E286" s="1" t="n">
+      <c r="E286" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="F286" s="1" t="n">
+      <c r="F286" s="7" t="n">
         <v>50</v>
       </c>
       <c r="L286" s="3" t="s">
@@ -6327,10 +6551,10 @@
       <c r="D287" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="E287" s="1" t="n">
+      <c r="E287" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="F287" s="1" t="n">
+      <c r="F287" s="7" t="n">
         <v>24</v>
       </c>
       <c r="L287" s="3" t="s">
@@ -6347,10 +6571,10 @@
       <c r="D288" s="0" t="s">
         <v>513</v>
       </c>
-      <c r="E288" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F288" s="1" t="n">
+      <c r="E288" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F288" s="7" t="n">
         <v>500</v>
       </c>
       <c r="L288" s="3" t="s">
@@ -6367,10 +6591,10 @@
       <c r="D289" s="0" t="s">
         <v>515</v>
       </c>
-      <c r="E289" s="1" t="n">
+      <c r="E289" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="F289" s="1" t="n">
+      <c r="F289" s="7" t="n">
         <v>16</v>
       </c>
       <c r="L289" s="3" t="s">
@@ -6387,10 +6611,10 @@
       <c r="D290" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="E290" s="1" t="n">
+      <c r="E290" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="F290" s="1" t="n">
+      <c r="F290" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L290" s="3" t="s">
@@ -6398,6 +6622,8 @@
       </c>
     </row>
     <row r="291" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E291" s="0"/>
+      <c r="F291" s="0"/>
       <c r="L291" s="0"/>
     </row>
     <row r="292" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6410,10 +6636,10 @@
       <c r="D292" s="0" t="s">
         <v>519</v>
       </c>
-      <c r="E292" s="1" t="n">
+      <c r="E292" s="7" t="n">
         <v>280</v>
       </c>
-      <c r="F292" s="1" t="n">
+      <c r="F292" s="7" t="n">
         <v>300</v>
       </c>
       <c r="L292" s="3" t="s">
@@ -6430,10 +6656,10 @@
       <c r="D293" s="0" t="s">
         <v>522</v>
       </c>
-      <c r="E293" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F293" s="1" t="n">
+      <c r="E293" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F293" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L293" s="3" t="s">
@@ -6450,10 +6676,10 @@
       <c r="D294" s="0" t="s">
         <v>555</v>
       </c>
-      <c r="E294" s="1" t="n">
+      <c r="E294" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="F294" s="1" t="n">
+      <c r="F294" s="7" t="n">
         <v>16</v>
       </c>
       <c r="L294" s="3" t="s">
@@ -6470,10 +6696,10 @@
       <c r="D295" s="0" t="s">
         <v>557</v>
       </c>
-      <c r="E295" s="1" t="n">
+      <c r="E295" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="F295" s="1" t="n">
+      <c r="F295" s="7" t="n">
         <v>25</v>
       </c>
       <c r="L295" s="3" t="s">
@@ -6520,12 +6746,12 @@
       </c>
     </row>
     <row r="302" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="12" t="s">
+      <c r="A302" s="11" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="20" t="s">
+      <c r="A304" s="18" t="s">
         <v>565</v>
       </c>
     </row>

</xml_diff>